<commit_message>
Added 0 values for MT+ in stream_gradient
</commit_message>
<xml_diff>
--- a/fmri/keuka_brain_behavior_analyses/dan/MNH Dan Labels.xlsx
+++ b/fmri/keuka_brain_behavior_analyses/dan/MNH Dan Labels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Data_Analysis/clock_analysis/fmri/pfc_entropy/masks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexdombrovski/code/clock_analysis/fmri/keuka_brain_behavior_analyses/dan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8CC17A-2899-2C4F-9A5B-A1E73736782A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148C1A0C-842B-1D44-BFFF-F613DD536838}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{4C85E76D-9D4B-0A4F-8C8E-B362A5AD0849}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{4C85E76D-9D4B-0A4F-8C8E-B362A5AD0849}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="112">
   <si>
     <t>7Networks_RH_DorsAttn_ITG_r</t>
   </si>
@@ -370,9 +370,6 @@
   </si>
   <si>
     <t>ventro-dorsal from Sakreida L Middle Temporal Gyrus</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -746,7 +743,7 @@
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1541,8 +1538,8 @@
       <c r="H24">
         <v>1</v>
       </c>
-      <c r="I24" s="3" t="s">
-        <v>112</v>
+      <c r="I24" s="3">
+        <v>0</v>
       </c>
       <c r="L24">
         <v>0</v>
@@ -1570,8 +1567,8 @@
       <c r="H25">
         <v>1</v>
       </c>
-      <c r="I25" s="3" t="s">
-        <v>112</v>
+      <c r="I25" s="3">
+        <v>0</v>
       </c>
       <c r="L25">
         <v>0</v>
@@ -1599,8 +1596,8 @@
       <c r="H26" s="3">
         <v>1</v>
       </c>
-      <c r="I26" s="3" t="s">
-        <v>112</v>
+      <c r="I26" s="3">
+        <v>0</v>
       </c>
       <c r="L26">
         <v>0</v>
@@ -1628,8 +1625,8 @@
       <c r="H27" s="3">
         <v>1</v>
       </c>
-      <c r="I27" s="3" t="s">
-        <v>112</v>
+      <c r="I27" s="3">
+        <v>0</v>
       </c>
       <c r="J27" t="s">
         <v>111</v>

</xml_diff>

<commit_message>
Source space MEG time domain prototype
</commit_message>
<xml_diff>
--- a/fmri/keuka_brain_behavior_analyses/dan/MNH Dan Labels.xlsx
+++ b/fmri/keuka_brain_behavior_analyses/dan/MNH Dan Labels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10502"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexdombrovski/code/clock_analysis/fmri/keuka_brain_behavior_analyses/dan/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/localadmin/code/clock_analysis/fmri/keuka_brain_behavior_analyses/dan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCE1CCC-40C9-EF40-BB59-17636A22D7E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D0B6C6-630F-7E43-877B-93F8EE043CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{4C85E76D-9D4B-0A4F-8C8E-B362A5AD0849}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="42180" windowHeight="20500" xr2:uid="{4C85E76D-9D4B-0A4F-8C8E-B362A5AD0849}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="120">
   <si>
     <t>7Networks_RH_DorsAttn_ITG_r</t>
   </si>
@@ -382,6 +382,18 @@
   </si>
   <si>
     <t>L_5_MT/V5_MST</t>
+  </si>
+  <si>
+    <t>lobe</t>
+  </si>
+  <si>
+    <t>parietal</t>
+  </si>
+  <si>
+    <t>frontal</t>
+  </si>
+  <si>
+    <t>temporal</t>
   </si>
 </sst>
 </file>
@@ -752,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87C388DC-DB77-E441-979A-A4AA56C5B741}">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -769,7 +781,7 @@
     <col min="11" max="11" width="52.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -806,8 +818,11 @@
       <c r="L1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="M1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>137</v>
       </c>
@@ -844,8 +859,11 @@
       <c r="L2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>34</v>
       </c>
@@ -879,8 +897,11 @@
       <c r="L3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="M3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>147</v>
       </c>
@@ -914,8 +935,11 @@
       <c r="L4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="M4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>43</v>
       </c>
@@ -949,8 +973,11 @@
       <c r="L5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="M5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>35</v>
       </c>
@@ -984,8 +1011,11 @@
       <c r="L6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="M6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>139</v>
       </c>
@@ -1016,8 +1046,11 @@
       <c r="L7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="M7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>138</v>
       </c>
@@ -1048,8 +1081,11 @@
       <c r="L8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="M8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>36</v>
       </c>
@@ -1080,8 +1116,11 @@
       <c r="L9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="M9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>141</v>
       </c>
@@ -1112,8 +1151,11 @@
       <c r="L10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="M10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>38</v>
       </c>
@@ -1144,8 +1186,11 @@
       <c r="L11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>145</v>
       </c>
@@ -1176,8 +1221,11 @@
       <c r="L12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>41</v>
       </c>
@@ -1208,8 +1256,11 @@
       <c r="L13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="M13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>142</v>
       </c>
@@ -1240,8 +1291,11 @@
       <c r="L14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="M14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>33</v>
       </c>
@@ -1275,8 +1329,11 @@
       <c r="L15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="M15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>144</v>
       </c>
@@ -1307,8 +1364,11 @@
       <c r="L16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="M16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>40</v>
       </c>
@@ -1342,8 +1402,11 @@
       <c r="L17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="M17" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>140</v>
       </c>
@@ -1374,8 +1437,11 @@
       <c r="L18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="M18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>37</v>
       </c>
@@ -1406,8 +1472,11 @@
       <c r="L19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="M19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>143</v>
       </c>
@@ -1438,8 +1507,11 @@
       <c r="L20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="M20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>39</v>
       </c>
@@ -1470,8 +1542,11 @@
       <c r="L21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>146</v>
       </c>
@@ -1499,8 +1574,11 @@
       <c r="L22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M22" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>42</v>
       </c>
@@ -1528,8 +1606,11 @@
       <c r="L23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M23" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>135</v>
       </c>
@@ -1557,8 +1638,11 @@
       <c r="L24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M24" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>136</v>
       </c>
@@ -1586,8 +1670,11 @@
       <c r="L25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M25" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>31</v>
       </c>
@@ -1615,8 +1702,11 @@
       <c r="L26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>32</v>
       </c>
@@ -1647,8 +1737,11 @@
       <c r="L27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="M27" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>25</v>
       </c>
@@ -1659,7 +1752,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>128</v>
       </c>

</xml_diff>

<commit_message>
Updates to tabulate_brain_behavior for B-B geom_pointrange
</commit_message>
<xml_diff>
--- a/fmri/keuka_brain_behavior_analyses/dan/MNH Dan Labels.xlsx
+++ b/fmri/keuka_brain_behavior_analyses/dan/MNH Dan Labels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10502"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/localadmin/code/clock_analysis/fmri/keuka_brain_behavior_analyses/dan/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hallquist/Data_Analysis/clock_analysis/fmri/keuka_brain_behavior_analyses/dan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D0B6C6-630F-7E43-877B-93F8EE043CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4ED0BA-5612-4448-B585-2544A8514112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="42180" windowHeight="20500" xr2:uid="{4C85E76D-9D4B-0A4F-8C8E-B362A5AD0849}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21100" xr2:uid="{4C85E76D-9D4B-0A4F-8C8E-B362A5AD0849}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="135">
   <si>
     <t>7Networks_RH_DorsAttn_ITG_r</t>
   </si>
@@ -162,9 +162,6 @@
     <t>7Networks_LH_DorsAttn_PrCv</t>
   </si>
   <si>
-    <t>reaching peak</t>
-  </si>
-  <si>
     <t>Neurosynth: saccade; Astafiev MIP</t>
   </si>
   <si>
@@ -231,9 +228,6 @@
     <t>Neurosynth: saccade; Astafiev aLIP pIPS [monkey LIP/VIP], bridges into aIPS</t>
   </si>
   <si>
-    <t>Somatomotor</t>
-  </si>
-  <si>
     <t>L_FEF</t>
   </si>
   <si>
@@ -394,6 +388,57 @@
   </si>
   <si>
     <t>temporal</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>PPvd</t>
+  </si>
+  <si>
+    <t>PMv</t>
+  </si>
+  <si>
+    <t>PPo</t>
+  </si>
+  <si>
+    <t>FEF</t>
+  </si>
+  <si>
+    <t>PPdd</t>
+  </si>
+  <si>
+    <t>PMd</t>
+  </si>
+  <si>
+    <t>MT+</t>
+  </si>
+  <si>
+    <t>Paper_Region</t>
+  </si>
+  <si>
+    <t>SPL</t>
+  </si>
+  <si>
+    <t>MIP/PRR</t>
+  </si>
+  <si>
+    <t>VIP</t>
+  </si>
+  <si>
+    <t>LIP</t>
+  </si>
+  <si>
+    <t>AIP</t>
+  </si>
+  <si>
+    <t>PFt</t>
+  </si>
+  <si>
+    <t>PFt (maybe combine with AIP)</t>
+  </si>
+  <si>
+    <t>Visuomotor_5</t>
   </si>
 </sst>
 </file>
@@ -764,65 +809,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87C388DC-DB77-E441-979A-A4AA56C5B741}">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="39.6640625" customWidth="1"/>
     <col min="3" max="5" width="27.6640625" customWidth="1"/>
-    <col min="6" max="6" width="52.1640625" style="1" customWidth="1"/>
-    <col min="7" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="18" style="3" customWidth="1"/>
-    <col min="10" max="10" width="18" customWidth="1"/>
-    <col min="11" max="11" width="52.1640625" customWidth="1"/>
+    <col min="6" max="8" width="52.1640625" style="1" customWidth="1"/>
+    <col min="9" max="11" width="18" customWidth="1"/>
+    <col min="12" max="12" width="18" style="3" customWidth="1"/>
+    <col min="13" max="13" width="18" customWidth="1"/>
+    <col min="14" max="14" width="52.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="M1" t="s">
+        <v>95</v>
+      </c>
+      <c r="N1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="J1" t="s">
-        <v>97</v>
-      </c>
-      <c r="K1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" t="s">
-        <v>52</v>
-      </c>
-      <c r="M1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="P1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>137</v>
       </c>
@@ -833,37 +887,46 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I2" t="s">
+        <v>94</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>4</v>
+      </c>
+      <c r="L2" s="3">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
         <v>96</v>
       </c>
-      <c r="H2">
-        <v>3</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>98</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="L2">
+      <c r="N2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="O2">
         <v>0</v>
       </c>
-      <c r="M2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="P2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>34</v>
       </c>
@@ -874,34 +937,43 @@
         <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I3" t="s">
+        <v>94</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>4</v>
+      </c>
+      <c r="L3" s="3">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
         <v>96</v>
       </c>
-      <c r="H3">
-        <v>3</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>98</v>
-      </c>
-      <c r="L3">
+      <c r="O3">
         <v>0</v>
       </c>
-      <c r="M3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="P3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>147</v>
       </c>
@@ -912,34 +984,43 @@
         <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="H4" s="3">
+        <v>103</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="J4" s="3">
         <v>4</v>
       </c>
-      <c r="I4" s="3">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s">
-        <v>99</v>
-      </c>
-      <c r="L4">
+      <c r="K4" s="3">
+        <v>5</v>
+      </c>
+      <c r="L4" s="3">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>97</v>
+      </c>
+      <c r="O4">
         <v>0</v>
       </c>
-      <c r="M4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="P4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>43</v>
       </c>
@@ -950,34 +1031,43 @@
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G5" t="s">
-        <v>96</v>
-      </c>
-      <c r="H5">
+        <v>103</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I5" t="s">
+        <v>94</v>
+      </c>
+      <c r="J5">
         <v>4</v>
       </c>
-      <c r="I5" s="3">
-        <v>1</v>
-      </c>
-      <c r="J5" t="s">
-        <v>104</v>
-      </c>
-      <c r="L5">
+      <c r="K5">
+        <v>5</v>
+      </c>
+      <c r="L5" s="3">
+        <v>1</v>
+      </c>
+      <c r="M5" t="s">
+        <v>102</v>
+      </c>
+      <c r="O5">
         <v>0</v>
       </c>
-      <c r="M5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="P5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>35</v>
       </c>
@@ -988,34 +1078,43 @@
         <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G6" t="s">
-        <v>96</v>
-      </c>
-      <c r="H6">
+        <v>104</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I6" t="s">
+        <v>94</v>
+      </c>
+      <c r="J6">
         <v>3</v>
       </c>
-      <c r="I6" s="3">
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6" s="3">
         <v>2</v>
       </c>
-      <c r="J6" t="s">
-        <v>107</v>
-      </c>
-      <c r="L6">
+      <c r="M6" t="s">
+        <v>105</v>
+      </c>
+      <c r="O6">
         <v>0</v>
       </c>
-      <c r="M6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="P6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>139</v>
       </c>
@@ -1026,31 +1125,40 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="G7" t="s">
-        <v>96</v>
-      </c>
-      <c r="H7">
+        <v>84</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J7">
         <v>3</v>
       </c>
-      <c r="I7" s="3">
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7" s="3">
         <v>2</v>
       </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-      <c r="M7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>138</v>
       </c>
@@ -1061,31 +1169,40 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G8" t="s">
-        <v>96</v>
-      </c>
-      <c r="H8">
+        <v>91</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I8" t="s">
+        <v>94</v>
+      </c>
+      <c r="J8">
         <v>3</v>
       </c>
-      <c r="I8" s="3">
+      <c r="K8">
+        <v>4</v>
+      </c>
+      <c r="L8" s="3">
         <v>3</v>
       </c>
-      <c r="L8">
-        <v>1</v>
-      </c>
-      <c r="M8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>36</v>
       </c>
@@ -1096,31 +1213,40 @@
         <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G9" t="s">
-        <v>96</v>
-      </c>
-      <c r="H9">
+        <v>86</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I9" t="s">
+        <v>94</v>
+      </c>
+      <c r="J9">
         <v>3</v>
       </c>
-      <c r="I9" s="3">
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="L9" s="3">
         <v>3</v>
       </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="M9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>141</v>
       </c>
@@ -1131,31 +1257,40 @@
         <v>13</v>
       </c>
       <c r="D10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E10" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G10" t="s">
-        <v>102</v>
-      </c>
-      <c r="H10">
+      <c r="G10" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I10" t="s">
+        <v>100</v>
+      </c>
+      <c r="J10">
         <v>3</v>
       </c>
-      <c r="I10" s="3">
+      <c r="K10">
         <v>4</v>
       </c>
-      <c r="L10">
-        <v>1</v>
-      </c>
-      <c r="M10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="L10" s="3">
+        <v>4</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>38</v>
       </c>
@@ -1166,31 +1301,40 @@
         <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G11" t="s">
-        <v>102</v>
-      </c>
-      <c r="H11">
+        <v>76</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I11" t="s">
+        <v>100</v>
+      </c>
+      <c r="J11">
         <v>3</v>
       </c>
-      <c r="I11" s="3">
+      <c r="K11">
         <v>4</v>
       </c>
-      <c r="L11">
-        <v>1</v>
-      </c>
-      <c r="M11" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L11" s="3">
+        <v>4</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>145</v>
       </c>
@@ -1201,31 +1345,40 @@
         <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E12" t="s">
-        <v>67</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="H12" s="3">
+        <v>65</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="J12" s="3">
         <v>4</v>
       </c>
-      <c r="I12" s="3">
+      <c r="K12" s="3">
+        <v>5</v>
+      </c>
+      <c r="L12" s="3">
         <v>4</v>
       </c>
-      <c r="J12" t="s">
-        <v>101</v>
-      </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
       <c r="M12" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>41</v>
       </c>
@@ -1236,31 +1389,40 @@
         <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E13" t="s">
-        <v>66</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="H13" s="3">
+        <v>64</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="J13" s="3">
         <v>4</v>
       </c>
-      <c r="I13" s="3">
+      <c r="K13" s="3">
+        <v>5</v>
+      </c>
+      <c r="L13" s="3">
         <v>4</v>
       </c>
-      <c r="J13" t="s">
-        <v>100</v>
-      </c>
-      <c r="L13">
-        <v>1</v>
-      </c>
       <c r="M13" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>142</v>
       </c>
@@ -1271,31 +1433,40 @@
         <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="H14">
+        <v>43</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="J14">
         <v>2</v>
       </c>
-      <c r="I14" s="3">
+      <c r="K14">
+        <v>3</v>
+      </c>
+      <c r="L14" s="3">
         <v>5</v>
       </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-      <c r="M14" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>33</v>
       </c>
@@ -1306,34 +1477,43 @@
         <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="H15">
+        <v>60</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="J15">
         <v>2</v>
       </c>
-      <c r="I15" s="3">
+      <c r="K15">
+        <v>3</v>
+      </c>
+      <c r="L15" s="3">
         <v>5</v>
       </c>
-      <c r="K15" t="s">
-        <v>47</v>
-      </c>
-      <c r="L15">
-        <v>1</v>
-      </c>
-      <c r="M15" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="N15" t="s">
+        <v>46</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>144</v>
       </c>
@@ -1344,31 +1524,40 @@
         <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G16" t="s">
-        <v>95</v>
-      </c>
-      <c r="H16">
+        <v>82</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I16" t="s">
+        <v>93</v>
+      </c>
+      <c r="J16">
         <v>3</v>
       </c>
-      <c r="I16" s="3">
+      <c r="K16">
+        <v>2</v>
+      </c>
+      <c r="L16" s="3">
         <v>6</v>
       </c>
-      <c r="L16">
+      <c r="O16">
         <v>0</v>
       </c>
-      <c r="M16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="P16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>40</v>
       </c>
@@ -1379,34 +1568,43 @@
         <v>19</v>
       </c>
       <c r="D17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E17" t="s">
-        <v>81</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G17" t="s">
-        <v>95</v>
-      </c>
-      <c r="H17">
+      <c r="G17" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I17" t="s">
+        <v>93</v>
+      </c>
+      <c r="J17">
         <v>3</v>
       </c>
-      <c r="I17" s="3">
+      <c r="K17">
+        <v>2</v>
+      </c>
+      <c r="L17" s="3">
         <v>6</v>
       </c>
-      <c r="K17" t="s">
-        <v>79</v>
-      </c>
-      <c r="L17">
+      <c r="N17" t="s">
+        <v>77</v>
+      </c>
+      <c r="O17">
         <v>0</v>
       </c>
-      <c r="M17" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="P17" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>140</v>
       </c>
@@ -1417,31 +1615,40 @@
         <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G18" t="s">
-        <v>95</v>
-      </c>
-      <c r="H18">
+        <v>44</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I18" t="s">
+        <v>93</v>
+      </c>
+      <c r="J18">
         <v>2</v>
       </c>
-      <c r="I18" s="3">
+      <c r="K18">
+        <v>3</v>
+      </c>
+      <c r="L18" s="3">
         <v>7</v>
       </c>
-      <c r="L18">
-        <v>1</v>
-      </c>
-      <c r="M18" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>37</v>
       </c>
@@ -1452,31 +1659,40 @@
         <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G19" t="s">
-        <v>95</v>
-      </c>
-      <c r="H19">
+        <v>42</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I19" t="s">
+        <v>93</v>
+      </c>
+      <c r="J19">
         <v>2</v>
       </c>
-      <c r="I19" s="3">
+      <c r="K19">
+        <v>3</v>
+      </c>
+      <c r="L19" s="3">
         <v>7</v>
       </c>
-      <c r="L19">
-        <v>1</v>
-      </c>
-      <c r="M19" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>143</v>
       </c>
@@ -1487,31 +1703,40 @@
         <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G20" t="s">
-        <v>95</v>
-      </c>
-      <c r="H20">
+        <v>73</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I20" t="s">
+        <v>93</v>
+      </c>
+      <c r="J20">
         <v>3</v>
       </c>
-      <c r="I20" s="3">
+      <c r="K20">
+        <v>2</v>
+      </c>
+      <c r="L20" s="3">
         <v>8</v>
       </c>
-      <c r="L20">
-        <v>1</v>
-      </c>
-      <c r="M20" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>39</v>
       </c>
@@ -1522,31 +1747,40 @@
         <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G21" t="s">
-        <v>95</v>
-      </c>
-      <c r="H21">
+        <v>75</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I21" t="s">
+        <v>93</v>
+      </c>
+      <c r="J21">
         <v>3</v>
       </c>
-      <c r="I21" s="3">
+      <c r="K21">
+        <v>2</v>
+      </c>
+      <c r="L21" s="3">
         <v>8</v>
       </c>
-      <c r="L21">
-        <v>1</v>
-      </c>
-      <c r="M21" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>146</v>
       </c>
@@ -1557,28 +1791,37 @@
         <v>23</v>
       </c>
       <c r="D22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E22" t="s">
-        <v>72</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="H22" s="3">
+        <v>70</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="J22" s="3">
         <v>4</v>
       </c>
-      <c r="I22" s="3">
+      <c r="K22" s="3">
+        <v>5</v>
+      </c>
+      <c r="L22" s="3">
         <v>8</v>
       </c>
-      <c r="L22">
-        <v>1</v>
-      </c>
-      <c r="M22" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>42</v>
       </c>
@@ -1589,28 +1832,37 @@
         <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E23" t="s">
-        <v>73</v>
-      </c>
-      <c r="G23" t="s">
-        <v>95</v>
-      </c>
-      <c r="H23">
+        <v>71</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I23" t="s">
+        <v>93</v>
+      </c>
+      <c r="J23">
         <v>4</v>
       </c>
-      <c r="I23" s="3">
+      <c r="K23">
+        <v>5</v>
+      </c>
+      <c r="L23" s="3">
         <v>8</v>
       </c>
-      <c r="L23">
-        <v>1</v>
-      </c>
-      <c r="M23" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>135</v>
       </c>
@@ -1621,28 +1873,37 @@
         <v>1</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="G24" t="s">
-        <v>109</v>
-      </c>
-      <c r="H24">
-        <v>1</v>
-      </c>
-      <c r="I24" s="3">
+        <v>110</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I24" t="s">
+        <v>107</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24" s="3">
         <v>0</v>
       </c>
-      <c r="L24">
+      <c r="O24">
         <v>0</v>
       </c>
-      <c r="M24" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>136</v>
       </c>
@@ -1653,28 +1914,37 @@
         <v>3</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="G25" t="s">
-        <v>109</v>
-      </c>
-      <c r="H25">
-        <v>1</v>
-      </c>
-      <c r="I25" s="3">
+        <v>111</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I25" t="s">
+        <v>107</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25" s="3">
         <v>0</v>
       </c>
-      <c r="L25">
+      <c r="O25">
         <v>0</v>
       </c>
-      <c r="M25" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P25" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>31</v>
       </c>
@@ -1685,28 +1955,37 @@
         <v>1</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="H26" s="3">
-        <v>1</v>
-      </c>
-      <c r="I26" s="3">
+        <v>112</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J26" s="3">
+        <v>1</v>
+      </c>
+      <c r="K26" s="3">
+        <v>1</v>
+      </c>
+      <c r="L26" s="3">
         <v>0</v>
       </c>
-      <c r="L26">
+      <c r="O26">
         <v>0</v>
       </c>
-      <c r="M26" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>32</v>
       </c>
@@ -1717,55 +1996,42 @@
         <v>3</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="G27" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J27" s="3">
+        <v>1</v>
+      </c>
+      <c r="K27" s="3">
+        <v>1</v>
+      </c>
+      <c r="L27" s="3">
+        <v>0</v>
+      </c>
+      <c r="M27" t="s">
         <v>109</v>
       </c>
-      <c r="H27" s="3">
-        <v>1</v>
-      </c>
-      <c r="I27" s="3">
+      <c r="O27">
         <v>0</v>
       </c>
-      <c r="J27" t="s">
-        <v>111</v>
-      </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-      <c r="M27" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>25</v>
-      </c>
-      <c r="B28" t="s">
-        <v>65</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>128</v>
-      </c>
-      <c r="B29" t="s">
-        <v>65</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>42</v>
+      <c r="P27" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L29">
-    <sortCondition ref="I2:I29"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O27">
+    <sortCondition ref="L2:L27"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add DAN 400 labels
</commit_message>
<xml_diff>
--- a/fmri/keuka_brain_behavior_analyses/dan/MNH Dan Labels.xlsx
+++ b/fmri/keuka_brain_behavior_analyses/dan/MNH Dan Labels.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hallquist/Data_Analysis/clock_analysis/fmri/keuka_brain_behavior_analyses/dan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4ED0BA-5612-4448-B585-2544A8514112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F992D2-F3FF-3D48-9D33-7D81C23C4461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21100" xr2:uid="{4C85E76D-9D4B-0A4F-8C8E-B362A5AD0849}"/>
   </bookViews>
@@ -811,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87C388DC-DB77-E441-979A-A4AA56C5B741}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="160" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -878,193 +878,181 @@
     </row>
     <row r="2" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>137</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>67</v>
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>112</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="I2" t="s">
-        <v>94</v>
-      </c>
-      <c r="J2">
-        <v>3</v>
-      </c>
-      <c r="K2">
-        <v>4</v>
+        <v>125</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J2" s="3">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3">
+        <v>1</v>
       </c>
       <c r="L2" s="3">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
-        <v>96</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>58</v>
+        <v>3</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="I3" t="s">
-        <v>94</v>
-      </c>
-      <c r="J3">
-        <v>3</v>
-      </c>
-      <c r="K3">
-        <v>4</v>
+        <v>125</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J3" s="3">
+        <v>1</v>
+      </c>
+      <c r="K3" s="3">
+        <v>1</v>
       </c>
       <c r="L3" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="O3">
         <v>0</v>
       </c>
       <c r="P3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+      <c r="L4" s="3">
+        <v>5</v>
+      </c>
+      <c r="N4" t="s">
+        <v>46</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>147</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="J4" s="3">
-        <v>4</v>
-      </c>
-      <c r="K4" s="3">
-        <v>5</v>
-      </c>
-      <c r="L4" s="3">
-        <v>1</v>
-      </c>
-      <c r="M4" t="s">
-        <v>97</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="E5" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>103</v>
+        <v>58</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I5" t="s">
         <v>94</v>
       </c>
       <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5">
         <v>4</v>
       </c>
-      <c r="K5">
-        <v>5</v>
-      </c>
       <c r="L5" s="3">
         <v>1</v>
       </c>
       <c r="M5" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="34" x14ac:dyDescent="0.2">
@@ -1114,27 +1102,27 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>139</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="E7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>119</v>
@@ -1149,7 +1137,7 @@
         <v>4</v>
       </c>
       <c r="L7" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O7">
         <v>1</v>
@@ -1158,42 +1146,42 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>138</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I8" t="s">
+        <v>93</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>3</v>
+      </c>
+      <c r="L8" s="3">
         <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>83</v>
-      </c>
-      <c r="E8" t="s">
-        <v>88</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="I8" t="s">
-        <v>94</v>
-      </c>
-      <c r="J8">
-        <v>3</v>
-      </c>
-      <c r="K8">
-        <v>4</v>
-      </c>
-      <c r="L8" s="3">
-        <v>3</v>
       </c>
       <c r="O8">
         <v>1</v>
@@ -1204,31 +1192,31 @@
     </row>
     <row r="9" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A9">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
         <v>36</v>
       </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="E9" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="I9" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="J9">
         <v>3</v>
@@ -1237,7 +1225,7 @@
         <v>4</v>
       </c>
       <c r="L9" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O9">
         <v>1</v>
@@ -1248,40 +1236,40 @@
     </row>
     <row r="10" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>141</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="I10" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="J10">
         <v>3</v>
       </c>
       <c r="K10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L10" s="3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="O10">
         <v>1</v>
@@ -1292,43 +1280,46 @@
     </row>
     <row r="11" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A11">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
         <v>38</v>
       </c>
-      <c r="B11" t="s">
-        <v>36</v>
-      </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="E11" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="I11" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="J11">
         <v>3</v>
       </c>
       <c r="K11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L11" s="3">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="N11" t="s">
+        <v>77</v>
       </c>
       <c r="O11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P11" t="s">
         <v>115</v>
@@ -1336,19 +1327,19 @@
     </row>
     <row r="12" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>145</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
         <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>122</v>
@@ -1369,7 +1360,7 @@
         <v>4</v>
       </c>
       <c r="M12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="O12">
         <v>1</v>
@@ -1380,40 +1371,37 @@
     </row>
     <row r="13" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="E13" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="J13" s="3">
+        <v>124</v>
+      </c>
+      <c r="I13" t="s">
+        <v>93</v>
+      </c>
+      <c r="J13">
         <v>4</v>
       </c>
-      <c r="K13" s="3">
+      <c r="K13">
         <v>5</v>
       </c>
       <c r="L13" s="3">
-        <v>4</v>
-      </c>
-      <c r="M13" t="s">
-        <v>98</v>
+        <v>8</v>
       </c>
       <c r="O13">
         <v>1</v>
@@ -1424,178 +1412,175 @@
     </row>
     <row r="14" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>142</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>43</v>
+        <v>103</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>100</v>
+        <v>120</v>
+      </c>
+      <c r="I14" t="s">
+        <v>94</v>
       </c>
       <c r="J14">
+        <v>4</v>
+      </c>
+      <c r="K14">
+        <v>5</v>
+      </c>
+      <c r="L14" s="3">
+        <v>1</v>
+      </c>
+      <c r="M14" t="s">
+        <v>102</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>135</v>
+      </c>
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I15" t="s">
+        <v>107</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15" s="3">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>136</v>
+      </c>
+      <c r="B16" t="s">
         <v>2</v>
       </c>
-      <c r="K14">
+      <c r="C16" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="L14" s="3">
-        <v>5</v>
-      </c>
-      <c r="O14">
-        <v>1</v>
-      </c>
-      <c r="P14" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>33</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="J15">
-        <v>2</v>
-      </c>
-      <c r="K15">
-        <v>3</v>
-      </c>
-      <c r="L15" s="3">
-        <v>5</v>
-      </c>
-      <c r="N15" t="s">
-        <v>46</v>
-      </c>
-      <c r="O15">
-        <v>1</v>
-      </c>
-      <c r="P15" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>144</v>
-      </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" t="s">
-        <v>78</v>
-      </c>
-      <c r="E16" t="s">
-        <v>78</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>82</v>
+      <c r="D16" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>111</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="I16" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="J16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L16" s="3">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>40</v>
+        <v>137</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I17" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J17">
         <v>3</v>
       </c>
       <c r="K17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L17" s="3">
-        <v>6</v>
-      </c>
-      <c r="N17" t="s">
-        <v>77</v>
+        <v>1</v>
+      </c>
+      <c r="M17" t="s">
+        <v>96</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="O17">
         <v>0</v>
@@ -1604,42 +1589,42 @@
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="E18" t="s">
-        <v>53</v>
+        <v>88</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K18">
+        <v>4</v>
+      </c>
+      <c r="L18" s="3">
         <v>3</v>
-      </c>
-      <c r="L18" s="3">
-        <v>7</v>
       </c>
       <c r="O18">
         <v>1</v>
@@ -1648,42 +1633,42 @@
         <v>115</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>37</v>
+        <v>139</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="E19" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I19" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J19">
+        <v>3</v>
+      </c>
+      <c r="K19">
+        <v>4</v>
+      </c>
+      <c r="L19" s="3">
         <v>2</v>
-      </c>
-      <c r="K19">
-        <v>3</v>
-      </c>
-      <c r="L19" s="3">
-        <v>7</v>
       </c>
       <c r="O19">
         <v>1</v>
@@ -1692,27 +1677,27 @@
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="E20" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>123</v>
@@ -1721,13 +1706,13 @@
         <v>93</v>
       </c>
       <c r="J20">
+        <v>2</v>
+      </c>
+      <c r="K20">
         <v>3</v>
       </c>
-      <c r="K20">
-        <v>2</v>
-      </c>
       <c r="L20" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O20">
         <v>1</v>
@@ -1738,40 +1723,40 @@
     </row>
     <row r="21" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>39</v>
+        <v>141</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="E21" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I21" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="J21">
         <v>3</v>
       </c>
       <c r="K21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L21" s="3">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="O21">
         <v>1</v>
@@ -1782,75 +1767,81 @@
     </row>
     <row r="22" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D22" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="E22" t="s">
-        <v>70</v>
+        <v>54</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="J22" s="3">
-        <v>4</v>
-      </c>
-      <c r="K22" s="3">
+        <v>100</v>
+      </c>
+      <c r="J22">
+        <v>2</v>
+      </c>
+      <c r="K22">
+        <v>3</v>
+      </c>
+      <c r="L22" s="3">
         <v>5</v>
       </c>
-      <c r="L22" s="3">
-        <v>8</v>
-      </c>
       <c r="O22">
         <v>1</v>
       </c>
       <c r="P22" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>42</v>
+        <v>143</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D23" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E23" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I23" t="s">
         <v>93</v>
       </c>
       <c r="J23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K23">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L23" s="3">
         <v>8</v>
@@ -1859,179 +1850,188 @@
         <v>1</v>
       </c>
       <c r="P23" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="B24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>110</v>
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" t="s">
+        <v>78</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I24" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="J24">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L24" s="3">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O24">
         <v>0</v>
       </c>
       <c r="P24" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="B25" t="s">
-        <v>2</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>111</v>
+        <v>20</v>
+      </c>
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" t="s">
+        <v>65</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I25" t="s">
-        <v>107</v>
-      </c>
-      <c r="J25">
-        <v>1</v>
-      </c>
-      <c r="K25">
-        <v>1</v>
+        <v>122</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="J25" s="3">
+        <v>4</v>
+      </c>
+      <c r="K25" s="3">
+        <v>5</v>
       </c>
       <c r="L25" s="3">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="M25" t="s">
+        <v>99</v>
       </c>
       <c r="O25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>31</v>
+        <v>146</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>112</v>
+        <v>23</v>
+      </c>
+      <c r="D26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" t="s">
+        <v>70</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="J26" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K26" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L26" s="3">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>32</v>
+        <v>147</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>3</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>113</v>
+        <v>25</v>
+      </c>
+      <c r="D27" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" t="s">
+        <v>68</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="J27" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K27" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L27" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M27" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="O27">
         <v>0</v>
       </c>
       <c r="P27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O27">
-    <sortCondition ref="L2:L27"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P27">
+    <sortCondition ref="A2:A27"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>